<commit_message>
Documentação: requisitos e mockup
</commit_message>
<xml_diff>
--- a/doc/02 - Gráfico de Gantt.xlsx
+++ b/doc/02 - Gráfico de Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8cca93f32cb85d0/UTFPR/2021-02/OP63L - Desenvolvimento de Aplicações para Dispositivos Móveis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{CB3DBB2D-5E21-4411-AD54-17263BB720A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3DEB506-DF02-461C-8EF5-577F8DDA201E}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="8_{CB3DBB2D-5E21-4411-AD54-17263BB720A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9358C9DE-9759-42AF-9879-77639E8CE56C}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="8250" windowWidth="15375" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planejador de Projetos" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -403,6 +403,21 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="13"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="39">
@@ -884,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -954,6 +969,15 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -990,11 +1014,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1059,6 +1080,35 @@
     <cellStyle name="Vírgula" xfId="19" builtinId="3" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1170,35 +1220,6 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1448,7 +1469,7 @@
   <dimension ref="B1:BO17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1475,13 +1496,13 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="2:67" ht="21.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1489,74 +1510,74 @@
         <v>3</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="33"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="36"/>
       <c r="R2" s="17"/>
-      <c r="S2" s="31" t="s">
+      <c r="S2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="33"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="36"/>
       <c r="W2" s="18"/>
-      <c r="X2" s="23" t="s">
+      <c r="X2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="34"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="37"/>
       <c r="AC2" s="19"/>
-      <c r="AD2" s="23" t="s">
+      <c r="AD2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="34"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="37"/>
       <c r="AL2" s="20"/>
-      <c r="AM2" s="23" t="s">
+      <c r="AM2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="24"/>
-      <c r="AQ2" s="24"/>
-      <c r="AR2" s="24"/>
-      <c r="AS2" s="24"/>
-      <c r="AT2" s="24"/>
-      <c r="AU2" s="24"/>
-      <c r="AV2" s="24"/>
-      <c r="AW2" s="24"/>
-      <c r="AX2" s="24"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+      <c r="AR2" s="27"/>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="40.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1583,12 +1604,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1907,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1918,12 +1939,16 @@
         <v>3</v>
       </c>
       <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1938,7 +1963,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="8">
+      <c r="G13" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1991,47 +2016,47 @@
       </c>
     </row>
     <row r="17" spans="7:21" ht="57.75" x14ac:dyDescent="0.3">
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="23">
         <v>44469</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="23">
         <v>44476</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="23">
         <v>44483</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="23">
         <v>44490</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="23">
         <v>44497</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="23">
         <v>44504</v>
       </c>
-      <c r="N17" s="35">
+      <c r="N17" s="23">
         <v>44511</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="23">
         <v>44518</v>
       </c>
-      <c r="P17" s="35">
+      <c r="P17" s="23">
         <v>44525</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="23">
         <v>44532</v>
       </c>
-      <c r="R17" s="35">
+      <c r="R17" s="23">
         <v>44539</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="23">
         <v>44546</v>
       </c>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2050,38 +2075,38 @@
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
   <conditionalFormatting sqref="H5:BO16">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>PorcentagemConcluída</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>PercentualConcluídoAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>Real</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>RealAlém</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>Plano</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>H$4=período_selecionado</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:BO17">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>H$4=período_selecionado</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>